<commit_message>
adjust depthshallow to gain ~25% speedup
</commit_message>
<xml_diff>
--- a/analysis/version87-debug and endgame.xlsx
+++ b/analysis/version87-debug and endgame.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11660" yWindow="0" windowWidth="25600" windowHeight="13860" tabRatio="500"/>
+    <workbookView xWindow="13980" yWindow="0" windowWidth="25600" windowHeight="13860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -490,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1773,8 +1773,8 @@
       </c>
       <c r="C67"/>
       <c r="D67">
-        <f>AVERAGE(D7:D44)</f>
-        <v>597.77368421052631</v>
+        <f>AVERAGE(D7:D46)</f>
+        <v>579.11</v>
       </c>
       <c r="E67" s="1">
         <f>AVERAGE(E7:E44)</f>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="D69">
         <f>D67/A67</f>
-        <v>0.90099091389570074</v>
+        <v>0.87286018426060252</v>
       </c>
       <c r="E69">
         <f>E67/B67</f>

</xml_diff>